<commit_message>
Modifs mineures conversion hexa/deci CAN
</commit_message>
<xml_diff>
--- a/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
+++ b/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F710D52-A753-46E4-B6D9-4FFBBEC73F28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F2761D-9E54-40E5-8F92-87E2DFE73E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,6 +238,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +524,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="D2:G2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,10 +541,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="4"/>
       <c r="D1" t="s">
         <v>2</v>
       </c>
@@ -557,10 +560,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>53</v>
@@ -582,9 +585,9 @@
       <c r="B3" s="1">
         <v>2000</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f>DEC2HEX(B3)</f>
-        <v>7D0</v>
+      <c r="C3" s="1">
+        <f>HEX2DEC(B3)</f>
+        <v>8192</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -603,9 +606,9 @@
       <c r="B4" s="1">
         <v>2001</v>
       </c>
-      <c r="C4" s="1" t="str">
-        <f t="shared" ref="C4:C14" si="0">DEC2HEX(B4)</f>
-        <v>7D1</v>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C16" si="0">HEX2DEC(B4)</f>
+        <v>8193</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -624,9 +627,9 @@
       <c r="B5" s="1">
         <v>2002</v>
       </c>
-      <c r="C5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>7D2</v>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>8194</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -645,9 +648,9 @@
       <c r="B6" s="1">
         <v>2003</v>
       </c>
-      <c r="C6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>7D3</v>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>8195</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -666,9 +669,9 @@
       <c r="B7" s="1">
         <v>2004</v>
       </c>
-      <c r="C7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>7D4</v>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>8196</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -687,9 +690,9 @@
       <c r="B8" s="1">
         <v>2005</v>
       </c>
-      <c r="C8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>7D5</v>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>8197</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -708,9 +711,9 @@
       <c r="B9" s="1">
         <v>2006</v>
       </c>
-      <c r="C9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>7D6</v>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>8198</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -729,9 +732,9 @@
       <c r="B10" s="1">
         <v>2007</v>
       </c>
-      <c r="C10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>7D7</v>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>8199</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -742,6 +745,9 @@
       <c r="F10" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -750,9 +756,9 @@
       <c r="B12" s="1">
         <v>1000</v>
       </c>
-      <c r="C12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3E8</v>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>4096</v>
       </c>
       <c r="D12" t="s">
         <v>43</v>
@@ -765,9 +771,9 @@
       <c r="B13" s="1">
         <v>1001</v>
       </c>
-      <c r="C13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3E9</v>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>4097</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -783,9 +789,9 @@
       <c r="B14" s="1">
         <v>1002</v>
       </c>
-      <c r="C14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>3EA</v>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>4098</v>
       </c>
       <c r="D14" t="s">
         <v>44</v>
@@ -796,6 +802,9 @@
       <c r="H14" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -804,9 +813,9 @@
       <c r="B16" s="1">
         <v>1100</v>
       </c>
-      <c r="C16" s="1" t="str">
-        <f>DEC2HEX(B16)</f>
-        <v>44C</v>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>4352</v>
       </c>
       <c r="D16" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Ménage et adaptation du code 2019 à 2020
</commit_message>
<xml_diff>
--- a/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
+++ b/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
@@ -172,7 +172,7 @@
     <t xml:space="preserve">Neutre</t>
   </si>
   <si>
-    <t xml:space="preserve">// 0x11 0x11 0x11 0x11 0x11 0x11 0x11 0x11</t>
+    <t xml:space="preserve">// 0x11 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
   </si>
   <si>
     <t xml:space="preserve">MAJ</t>
@@ -319,7 +319,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -328,7 +328,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.79"/>
   </cols>

</xml_diff>

<commit_message>
Modif code carte arrière
</commit_message>
<xml_diff>
--- a/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
+++ b/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>System</t>
   </si>
@@ -180,12 +180,6 @@
     <t>MAJ</t>
   </si>
   <si>
-    <t>Launch</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
     <t>W/D</t>
   </si>
   <si>
@@ -205,6 +199,9 @@
   </si>
   <si>
     <t>Auto</t>
+  </si>
+  <si>
+    <t>Launch Control</t>
   </si>
 </sst>
 </file>
@@ -248,14 +245,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,13 +587,13 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
@@ -608,10 +605,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="4"/>
       <c r="D1" t="s">
         <v>2</v>
       </c>
@@ -626,22 +623,22 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -649,10 +646,10 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>2000</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <f t="shared" ref="C3:C10" si="0">HEX2DEC(B3)</f>
         <v>8192</v>
       </c>
@@ -670,10 +667,10 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>2001</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>8193</v>
       </c>
@@ -691,10 +688,10 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>2002</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>8194</v>
       </c>
@@ -712,10 +709,10 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>2003</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>8195</v>
       </c>
@@ -733,10 +730,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>2004</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>8196</v>
       </c>
@@ -754,10 +751,10 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>2005</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>8197</v>
       </c>
@@ -775,10 +772,10 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>2006</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>8198</v>
       </c>
@@ -796,10 +793,10 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>2007</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>8199</v>
       </c>
@@ -814,24 +811,24 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="3"/>
       <c r="F12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1">
         <v>1001</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <f t="shared" ref="C13:C18" si="1">HEX2DEC(B13)</f>
         <v>4097</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F13" t="s">
@@ -842,15 +839,15 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1">
         <v>1002</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <f t="shared" si="1"/>
         <v>4098</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="F14" t="s">
@@ -861,97 +858,88 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1">
         <v>1003</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <f t="shared" si="1"/>
         <v>4099</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>52</v>
+      <c r="D15" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2">
-        <v>1004</v>
-      </c>
-      <c r="C16" s="2">
-        <f t="shared" si="1"/>
-        <v>4100</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1">
         <v>1005</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <f t="shared" si="1"/>
         <v>4101</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>54</v>
+      <c r="D17" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1">
         <v>1006</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <f t="shared" si="1"/>
         <v>4102</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>55</v>
+      <c r="D18" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1">
         <v>1008</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <f>HEX2DEC(B20)</f>
         <v>4104</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>56</v>
+      <c r="D20" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="A22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1">
         <v>1100</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <f>HEX2DEC(B22)</f>
         <v>4352</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" t="s">
         <v>58</v>
-      </c>
-      <c r="E22" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code carte arrière avec interruptions et maj excel adress CAN
</commit_message>
<xml_diff>
--- a/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
+++ b/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobau\Documents\EPSA\Ressources2020\EL_Electrical\Dashboard controller\Arduino\Bus Can ID\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>System</t>
   </si>
@@ -202,12 +207,15 @@
   </si>
   <si>
     <t>Launch Control</t>
+  </si>
+  <si>
+    <t>Traction control</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,6 +267,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -587,21 +603,21 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -642,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -666,7 +682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2001</v>
       </c>
@@ -687,7 +703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2002</v>
       </c>
@@ -708,7 +724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2003</v>
       </c>
@@ -729,7 +745,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>2004</v>
       </c>
@@ -750,7 +766,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>2005</v>
       </c>
@@ -771,7 +787,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>2006</v>
       </c>
@@ -792,7 +808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>2007</v>
       </c>
@@ -810,7 +826,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
@@ -819,7 +835,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1">
         <v>1001</v>
@@ -838,7 +854,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="1">
         <v>1002</v>
@@ -857,7 +873,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1">
         <v>1003</v>
@@ -870,11 +886,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="B16" s="1">
+        <v>1004</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4100</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="1">
         <v>1005</v>
@@ -887,7 +911,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="1">
         <v>1006</v>
@@ -900,11 +924,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="1">
         <v>1008</v>
@@ -917,11 +941,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
MAJ carte avant correction bug et changement CAN
</commit_message>
<xml_diff>
--- a/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
+++ b/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
@@ -5,16 +5,16 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobau\Documents\EPSA\Ressources2020\EL_Electrical\Dashboard controller\Arduino\Bus Can ID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lecoc\Desktop\EPSA\Ressource 2020\EL_Electrical\Dashboard controller\Arduino\Bus Can ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-465" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-468" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>System</t>
   </si>
@@ -164,33 +164,15 @@
     <t>Carte avant</t>
   </si>
   <si>
-    <t>// MSG:</t>
-  </si>
-  <si>
     <t>Homing</t>
   </si>
   <si>
-    <t xml:space="preserve">// 0x00 0x00 0x00 0x00 0x00 0x00 0x00 0x00 </t>
-  </si>
-  <si>
-    <t>pas de MAJ</t>
-  </si>
-  <si>
     <t>Neutre</t>
   </si>
   <si>
-    <t>// 0x11 0x00 0x00 0x00 0x00 0x00 0x00 0x00</t>
-  </si>
-  <si>
-    <t>MAJ</t>
-  </si>
-  <si>
     <t>W/D</t>
   </si>
   <si>
-    <t>Log</t>
-  </si>
-  <si>
     <t>Log RaceCapture</t>
   </si>
   <si>
@@ -210,12 +192,15 @@
   </si>
   <si>
     <t>Traction control</t>
+  </si>
+  <si>
+    <t>LOG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -600,24 +585,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="3" width="8.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="1025" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -638,7 +623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -658,7 +643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -682,7 +667,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2001</v>
       </c>
@@ -703,7 +688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>2002</v>
       </c>
@@ -724,7 +709,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2003</v>
       </c>
@@ -745,7 +730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>2004</v>
       </c>
@@ -766,7 +751,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>2005</v>
       </c>
@@ -787,7 +772,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>2006</v>
       </c>
@@ -808,7 +793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>2007</v>
       </c>
@@ -826,144 +811,81 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>1001</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ref="C13:C18" si="1">HEX2DEC(B13)</f>
+        <f>HEX2DEC(B13)</f>
         <v>4097</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
         <v>46</v>
       </c>
       <c r="F13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" t="s">
         <v>47</v>
       </c>
-      <c r="H13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="1">
-        <v>1002</v>
-      </c>
-      <c r="C14" s="1">
-        <f t="shared" si="1"/>
-        <v>4098</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="1">
-        <v>1003</v>
-      </c>
-      <c r="C15" s="1">
-        <f t="shared" si="1"/>
-        <v>4099</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="1">
-        <v>1004</v>
+        <v>1008</v>
       </c>
       <c r="C16" s="1">
-        <v>4100</v>
+        <f>HEX2DEC(B16)</f>
+        <v>4104</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="1">
-        <v>1005</v>
-      </c>
-      <c r="C17" s="1">
-        <f t="shared" si="1"/>
-        <v>4101</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1100</v>
+      </c>
+      <c r="C18" s="1">
+        <f>HEX2DEC(B18)</f>
+        <v>4352</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1">
-        <v>1006</v>
-      </c>
-      <c r="C18" s="1">
-        <f t="shared" si="1"/>
-        <v>4102</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="1">
-        <v>1008</v>
-      </c>
-      <c r="C20" s="1">
-        <f>HEX2DEC(B20)</f>
-        <v>4104</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1100</v>
-      </c>
-      <c r="C22" s="1">
-        <f>HEX2DEC(B22)</f>
-        <v>4352</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debug code avant/arrière pour le CAN
</commit_message>
<xml_diff>
--- a/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
+++ b/EL_Electrical/Dashboard controller/Arduino/Bus Can ID/Bus CAN ID List.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lecoc\Desktop\EPSA\Ressource 2020\EL_Electrical\Dashboard controller\Arduino\Bus Can ID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\Documents\EPSA\Ressources2020\EL_Electrical\Dashboard controller\Arduino\Bus Can ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14753754-5165-4FD2-A29B-8F5DF2E797DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-468" windowWidth="33600" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -200,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -584,25 +585,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="1025" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -643,7 +644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -667,7 +668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2001</v>
       </c>
@@ -688,7 +689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2002</v>
       </c>
@@ -709,7 +710,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>2003</v>
       </c>
@@ -730,7 +731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>2004</v>
       </c>
@@ -751,7 +752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>2005</v>
       </c>
@@ -772,7 +773,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>2006</v>
       </c>
@@ -793,7 +794,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>2007</v>
       </c>
@@ -811,18 +812,18 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
-        <v>1001</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1">
-        <f>HEX2DEC(B13)</f>
-        <v>4097</v>
+        <f t="shared" ref="C13:C17" si="1">HEX2DEC(B13)</f>
+        <v>256</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>45</v>
@@ -843,40 +844,40 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="1">
         <v>1008</v>
       </c>
       <c r="C16" s="1">
-        <f>HEX2DEC(B16)</f>
+        <f t="shared" si="1"/>
         <v>4104</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B18" s="1">
-        <v>1100</v>
+        <v>110</v>
       </c>
       <c r="C18" s="1">
         <f>HEX2DEC(B18)</f>
-        <v>4352</v>
+        <v>272</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>50</v>

</xml_diff>